<commit_message>
working more or less
Former-commit-id: fbf5789d3dc3c9881c88eb235f81eee660d0aa35
</commit_message>
<xml_diff>
--- a/db/dummydata/easyshipping/ez_seeder_local_charges.xlsx
+++ b/db/dummydata/easyshipping/ez_seeder_local_charges.xlsx
@@ -7,9 +7,10 @@
     <sheet state="visible" name="Kobe Port" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="Dalian Port" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="Chattanooga Port" sheetId="4" r:id="rId6"/>
-    <sheet state="visible" name="Copenhagen Railyard" sheetId="5" r:id="rId7"/>
-    <sheet state="visible" name="Hamburg Railyard" sheetId="6" r:id="rId8"/>
-    <sheet state="visible" name="Rotterdam Railyard" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="Miami Port" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="Copenhagen Railyard" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="Hamburg Railyard" sheetId="7" r:id="rId9"/>
+    <sheet state="visible" name="Rotterdam Railyard" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="69">
   <si>
     <t>EFFECTIVE_DATE</t>
   </si>
@@ -121,16 +122,19 @@
     <t>Handling RTM</t>
   </si>
   <si>
+    <t>HDL</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
     <t>PFU</t>
   </si>
   <si>
     <t>PER_CBM_TON</t>
   </si>
   <si>
-    <t>HDL</t>
-  </si>
-  <si>
-    <t>export</t>
+    <t>ONC</t>
   </si>
   <si>
     <t>Import Handling</t>
@@ -145,19 +149,16 @@
     <t>PER_SHIPMENT</t>
   </si>
   <si>
-    <t>economy</t>
-  </si>
-  <si>
-    <t>ONC</t>
-  </si>
-  <si>
-    <t>express</t>
-  </si>
-  <si>
     <t>Stabrand THC</t>
   </si>
   <si>
     <t>THC</t>
+  </si>
+  <si>
+    <t>economy</t>
+  </si>
+  <si>
+    <t>express</t>
   </si>
   <si>
     <t>Terminal Handling Cost</t>
@@ -312,11 +313,11 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
@@ -384,6 +385,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -495,41 +500,41 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="8">
         <f t="shared" ref="A2:A13" si="1">TODAY()</f>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B2" s="8">
         <f t="shared" ref="B2:B13" si="2">A2 + 365</f>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="11" t="s">
+      <c r="E2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="11">
+      <c r="K2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="12">
         <v>10.0</v>
       </c>
-      <c r="M2" s="11">
+      <c r="M2" s="12">
         <v>10.0</v>
       </c>
       <c r="N2" s="10"/>
@@ -537,7 +542,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
-      <c r="S2" s="11">
+      <c r="S2" s="12">
         <v>50.0</v>
       </c>
       <c r="T2" s="10"/>
@@ -553,42 +558,42 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="8">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B3" s="8">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C3" s="10"/>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="11" t="s">
+      <c r="E3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="11" t="s">
+      <c r="G3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>41</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
-      <c r="P3" s="11">
+      <c r="P3" s="12">
         <v>250.0</v>
       </c>
       <c r="Q3" s="10"/>
@@ -607,41 +612,41 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="8">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B4" s="8">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="D4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="G4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="11">
+      <c r="K4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="12">
         <v>10.0</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="12">
         <v>10.0</v>
       </c>
       <c r="N4" s="10"/>
@@ -649,7 +654,7 @@
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" s="11">
+      <c r="S4" s="12">
         <v>50.0</v>
       </c>
       <c r="T4" s="10"/>
@@ -665,42 +670,42 @@
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="8">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B5" s="8">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
-      <c r="P5" s="11">
+      <c r="P5" s="12">
         <v>250.0</v>
       </c>
       <c r="Q5" s="10"/>
@@ -719,24 +724,24 @@
     <row r="6">
       <c r="A6" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B6" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>25</v>
@@ -748,7 +753,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L6" s="14">
         <v>10.0</v>
@@ -777,24 +782,24 @@
     <row r="7">
       <c r="A7" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B7" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>25</v>
@@ -803,10 +808,10 @@
         <v>26</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
@@ -831,49 +836,49 @@
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="G8" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="11">
+      <c r="L8" s="12">
         <v>15.0</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="12">
         <v>15.0</v>
       </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
-      <c r="Q8" s="11"/>
+      <c r="Q8" s="12"/>
       <c r="R8" s="10"/>
-      <c r="S8" s="11">
+      <c r="S8" s="12">
         <v>50.0</v>
       </c>
       <c r="T8" s="10"/>
@@ -889,45 +894,45 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B9" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C9" s="10"/>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="11" t="s">
+      <c r="I9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>41</v>
+      <c r="K9" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="P9" s="11">
+      <c r="P9" s="12">
         <v>5.0</v>
       </c>
-      <c r="Q9" s="11"/>
+      <c r="Q9" s="12"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
@@ -943,45 +948,45 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B10" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="11" t="s">
+      <c r="I10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>41</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="11">
+      <c r="P10" s="12">
         <v>250.0</v>
       </c>
-      <c r="Q10" s="11"/>
+      <c r="Q10" s="12"/>
       <c r="R10" s="10"/>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
@@ -997,45 +1002,45 @@
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B11" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="11" t="s">
+      <c r="I11" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="11" t="s">
-        <v>41</v>
+      <c r="K11" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
-      <c r="P11" s="11">
+      <c r="P11" s="12">
         <v>20.0</v>
       </c>
-      <c r="Q11" s="11"/>
+      <c r="Q11" s="12"/>
       <c r="R11" s="10"/>
       <c r="S11" s="10"/>
       <c r="T11" s="10"/>
@@ -1051,49 +1056,49 @@
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B12" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" s="11">
+      <c r="L12" s="12">
         <v>5.0</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="12">
         <v>5.0</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
-      <c r="P12" s="11"/>
+      <c r="P12" s="12"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
-      <c r="S12" s="11">
+      <c r="S12" s="12">
         <v>5.0</v>
       </c>
       <c r="T12" s="10"/>
@@ -1109,35 +1114,35 @@
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B13" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
-      </c>
-      <c r="D13" s="11" t="s">
+        <v>43658</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>32</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>27</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L13" s="6">
         <v>10.0</v>
@@ -1164,7 +1169,7 @@
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="11"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1194,7 +1199,7 @@
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
@@ -1221,23 +1226,23 @@
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
-      <c r="S16" s="11"/>
+      <c r="S16" s="12"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
@@ -1251,20 +1256,20 @@
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
-      <c r="P17" s="11"/>
+      <c r="P17" s="12"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
@@ -1281,23 +1286,23 @@
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
-      <c r="S18" s="11"/>
+      <c r="S18" s="12"/>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
@@ -1311,20 +1316,20 @@
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="11"/>
+      <c r="P19" s="12"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
@@ -1341,23 +1346,23 @@
     <row r="20">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
-      <c r="S20" s="11"/>
+      <c r="S20" s="12"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10"/>
@@ -1371,20 +1376,20 @@
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="11"/>
+      <c r="P21" s="12"/>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
@@ -1402,19 +1407,19 @@
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="11"/>
+      <c r="P22" s="12"/>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
@@ -1487,7 +1492,7 @@
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="7"/>
-      <c r="D29" s="11"/>
+      <c r="D29" s="12"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="10"/>
@@ -30887,36 +30892,36 @@
     <row r="2">
       <c r="A2" s="7">
         <f t="shared" ref="A2:A4" si="1">TODAY()</f>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B2" s="7">
         <f t="shared" ref="B2:B4" si="2">A2 + 365</f>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="G2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="L2" s="14">
         <v>25.0</v>
@@ -30945,36 +30950,36 @@
     <row r="3">
       <c r="A3" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B3" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="E3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="G3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="L3" s="14">
         <v>50.0</v>
@@ -31003,36 +31008,36 @@
     <row r="4">
       <c r="A4" s="7">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B4" s="7">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="G4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="L4" s="14">
         <v>135.0</v>
@@ -31185,6 +31190,127 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+    </row>
+    <row r="2">
+      <c r="D2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" s="6">
+        <v>50.0</v>
+      </c>
+      <c r="T2" s="6">
+        <v>25.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -31295,11 +31421,11 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="23">
         <f t="shared" ref="A2:A9" si="1">TODAY()</f>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B2" s="23">
         <f t="shared" ref="B2:B9" si="2">A2 + 365</f>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E2" t="s">
         <v>57</v>
@@ -31308,7 +31434,7 @@
         <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
         <v>59</v>
@@ -31317,10 +31443,10 @@
         <v>60</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L2" s="6">
         <v>150.0</v>
@@ -31335,11 +31461,11 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B3" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E3" t="s">
         <v>61</v>
@@ -31357,10 +31483,10 @@
         <v>60</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P3" s="6">
         <v>250.0</v>
@@ -31369,11 +31495,11 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B4" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
@@ -31391,10 +31517,10 @@
         <v>60</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L4" s="6"/>
       <c r="P4" s="6">
@@ -31405,11 +31531,11 @@
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B5" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -31444,11 +31570,11 @@
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B6" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E6" t="s">
         <v>57</v>
@@ -31457,7 +31583,7 @@
         <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
         <v>59</v>
@@ -31466,10 +31592,10 @@
         <v>68</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L6" s="6">
         <v>150.0</v>
@@ -31484,11 +31610,11 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B7" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E7" t="s">
         <v>61</v>
@@ -31506,10 +31632,10 @@
         <v>68</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P7" s="6">
         <v>250.0</v>
@@ -31518,11 +31644,11 @@
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B8" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E8" t="s">
         <v>63</v>
@@ -31540,10 +31666,10 @@
         <v>68</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L8" s="6"/>
       <c r="P8" s="6">
@@ -31554,11 +31680,11 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B9" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -31588,1577 +31714,6 @@
       </c>
       <c r="S9" s="6">
         <v>166.0</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
-    <row r="161" ht="15.75" customHeight="1"/>
-    <row r="162" ht="15.75" customHeight="1"/>
-    <row r="163" ht="15.75" customHeight="1"/>
-    <row r="164" ht="15.75" customHeight="1"/>
-    <row r="165" ht="15.75" customHeight="1"/>
-    <row r="166" ht="15.75" customHeight="1"/>
-    <row r="167" ht="15.75" customHeight="1"/>
-    <row r="168" ht="15.75" customHeight="1"/>
-    <row r="169" ht="15.75" customHeight="1"/>
-    <row r="170" ht="15.75" customHeight="1"/>
-    <row r="171" ht="15.75" customHeight="1"/>
-    <row r="172" ht="15.75" customHeight="1"/>
-    <row r="173" ht="15.75" customHeight="1"/>
-    <row r="174" ht="15.75" customHeight="1"/>
-    <row r="175" ht="15.75" customHeight="1"/>
-    <row r="176" ht="15.75" customHeight="1"/>
-    <row r="177" ht="15.75" customHeight="1"/>
-    <row r="178" ht="15.75" customHeight="1"/>
-    <row r="179" ht="15.75" customHeight="1"/>
-    <row r="180" ht="15.75" customHeight="1"/>
-    <row r="181" ht="15.75" customHeight="1"/>
-    <row r="182" ht="15.75" customHeight="1"/>
-    <row r="183" ht="15.75" customHeight="1"/>
-    <row r="184" ht="15.75" customHeight="1"/>
-    <row r="185" ht="15.75" customHeight="1"/>
-    <row r="186" ht="15.75" customHeight="1"/>
-    <row r="187" ht="15.75" customHeight="1"/>
-    <row r="188" ht="15.75" customHeight="1"/>
-    <row r="189" ht="15.75" customHeight="1"/>
-    <row r="190" ht="15.75" customHeight="1"/>
-    <row r="191" ht="15.75" customHeight="1"/>
-    <row r="192" ht="15.75" customHeight="1"/>
-    <row r="193" ht="15.75" customHeight="1"/>
-    <row r="194" ht="15.75" customHeight="1"/>
-    <row r="195" ht="15.75" customHeight="1"/>
-    <row r="196" ht="15.75" customHeight="1"/>
-    <row r="197" ht="15.75" customHeight="1"/>
-    <row r="198" ht="15.75" customHeight="1"/>
-    <row r="199" ht="15.75" customHeight="1"/>
-    <row r="200" ht="15.75" customHeight="1"/>
-    <row r="201" ht="15.75" customHeight="1"/>
-    <row r="202" ht="15.75" customHeight="1"/>
-    <row r="203" ht="15.75" customHeight="1"/>
-    <row r="204" ht="15.75" customHeight="1"/>
-    <row r="205" ht="15.75" customHeight="1"/>
-    <row r="206" ht="15.75" customHeight="1"/>
-    <row r="207" ht="15.75" customHeight="1"/>
-    <row r="208" ht="15.75" customHeight="1"/>
-    <row r="209" ht="15.75" customHeight="1"/>
-    <row r="210" ht="15.75" customHeight="1"/>
-    <row r="211" ht="15.75" customHeight="1"/>
-    <row r="212" ht="15.75" customHeight="1"/>
-    <row r="213" ht="15.75" customHeight="1"/>
-    <row r="214" ht="15.75" customHeight="1"/>
-    <row r="215" ht="15.75" customHeight="1"/>
-    <row r="216" ht="15.75" customHeight="1"/>
-    <row r="217" ht="15.75" customHeight="1"/>
-    <row r="218" ht="15.75" customHeight="1"/>
-    <row r="219" ht="15.75" customHeight="1"/>
-    <row r="220" ht="15.75" customHeight="1"/>
-    <row r="221" ht="15.75" customHeight="1"/>
-    <row r="222" ht="15.75" customHeight="1"/>
-    <row r="223" ht="15.75" customHeight="1"/>
-    <row r="224" ht="15.75" customHeight="1"/>
-    <row r="225" ht="15.75" customHeight="1"/>
-    <row r="226" ht="15.75" customHeight="1"/>
-    <row r="227" ht="15.75" customHeight="1"/>
-    <row r="228" ht="15.75" customHeight="1"/>
-    <row r="229" ht="15.75" customHeight="1"/>
-    <row r="230" ht="15.75" customHeight="1"/>
-    <row r="231" ht="15.75" customHeight="1"/>
-    <row r="232" ht="15.75" customHeight="1"/>
-    <row r="233" ht="15.75" customHeight="1"/>
-    <row r="234" ht="15.75" customHeight="1"/>
-    <row r="235" ht="15.75" customHeight="1"/>
-    <row r="236" ht="15.75" customHeight="1"/>
-    <row r="237" ht="15.75" customHeight="1"/>
-    <row r="238" ht="15.75" customHeight="1"/>
-    <row r="239" ht="15.75" customHeight="1"/>
-    <row r="240" ht="15.75" customHeight="1"/>
-    <row r="241" ht="15.75" customHeight="1"/>
-    <row r="242" ht="15.75" customHeight="1"/>
-    <row r="243" ht="15.75" customHeight="1"/>
-    <row r="244" ht="15.75" customHeight="1"/>
-    <row r="245" ht="15.75" customHeight="1"/>
-    <row r="246" ht="15.75" customHeight="1"/>
-    <row r="247" ht="15.75" customHeight="1"/>
-    <row r="248" ht="15.75" customHeight="1"/>
-    <row r="249" ht="15.75" customHeight="1"/>
-    <row r="250" ht="15.75" customHeight="1"/>
-    <row r="251" ht="15.75" customHeight="1"/>
-    <row r="252" ht="15.75" customHeight="1"/>
-    <row r="253" ht="15.75" customHeight="1"/>
-    <row r="254" ht="15.75" customHeight="1"/>
-    <row r="255" ht="15.75" customHeight="1"/>
-    <row r="256" ht="15.75" customHeight="1"/>
-    <row r="257" ht="15.75" customHeight="1"/>
-    <row r="258" ht="15.75" customHeight="1"/>
-    <row r="259" ht="15.75" customHeight="1"/>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
-    <row r="263" ht="15.75" customHeight="1"/>
-    <row r="264" ht="15.75" customHeight="1"/>
-    <row r="265" ht="15.75" customHeight="1"/>
-    <row r="266" ht="15.75" customHeight="1"/>
-    <row r="267" ht="15.75" customHeight="1"/>
-    <row r="268" ht="15.75" customHeight="1"/>
-    <row r="269" ht="15.75" customHeight="1"/>
-    <row r="270" ht="15.75" customHeight="1"/>
-    <row r="271" ht="15.75" customHeight="1"/>
-    <row r="272" ht="15.75" customHeight="1"/>
-    <row r="273" ht="15.75" customHeight="1"/>
-    <row r="274" ht="15.75" customHeight="1"/>
-    <row r="275" ht="15.75" customHeight="1"/>
-    <row r="276" ht="15.75" customHeight="1"/>
-    <row r="277" ht="15.75" customHeight="1"/>
-    <row r="278" ht="15.75" customHeight="1"/>
-    <row r="279" ht="15.75" customHeight="1"/>
-    <row r="280" ht="15.75" customHeight="1"/>
-    <row r="281" ht="15.75" customHeight="1"/>
-    <row r="282" ht="15.75" customHeight="1"/>
-    <row r="283" ht="15.75" customHeight="1"/>
-    <row r="284" ht="15.75" customHeight="1"/>
-    <row r="285" ht="15.75" customHeight="1"/>
-    <row r="286" ht="15.75" customHeight="1"/>
-    <row r="287" ht="15.75" customHeight="1"/>
-    <row r="288" ht="15.75" customHeight="1"/>
-    <row r="289" ht="15.75" customHeight="1"/>
-    <row r="290" ht="15.75" customHeight="1"/>
-    <row r="291" ht="15.75" customHeight="1"/>
-    <row r="292" ht="15.75" customHeight="1"/>
-    <row r="293" ht="15.75" customHeight="1"/>
-    <row r="294" ht="15.75" customHeight="1"/>
-    <row r="295" ht="15.75" customHeight="1"/>
-    <row r="296" ht="15.75" customHeight="1"/>
-    <row r="297" ht="15.75" customHeight="1"/>
-    <row r="298" ht="15.75" customHeight="1"/>
-    <row r="299" ht="15.75" customHeight="1"/>
-    <row r="300" ht="15.75" customHeight="1"/>
-    <row r="301" ht="15.75" customHeight="1"/>
-    <row r="302" ht="15.75" customHeight="1"/>
-    <row r="303" ht="15.75" customHeight="1"/>
-    <row r="304" ht="15.75" customHeight="1"/>
-    <row r="305" ht="15.75" customHeight="1"/>
-    <row r="306" ht="15.75" customHeight="1"/>
-    <row r="307" ht="15.75" customHeight="1"/>
-    <row r="308" ht="15.75" customHeight="1"/>
-    <row r="309" ht="15.75" customHeight="1"/>
-    <row r="310" ht="15.75" customHeight="1"/>
-    <row r="311" ht="15.75" customHeight="1"/>
-    <row r="312" ht="15.75" customHeight="1"/>
-    <row r="313" ht="15.75" customHeight="1"/>
-    <row r="314" ht="15.75" customHeight="1"/>
-    <row r="315" ht="15.75" customHeight="1"/>
-    <row r="316" ht="15.75" customHeight="1"/>
-    <row r="317" ht="15.75" customHeight="1"/>
-    <row r="318" ht="15.75" customHeight="1"/>
-    <row r="319" ht="15.75" customHeight="1"/>
-    <row r="320" ht="15.75" customHeight="1"/>
-    <row r="321" ht="15.75" customHeight="1"/>
-    <row r="322" ht="15.75" customHeight="1"/>
-    <row r="323" ht="15.75" customHeight="1"/>
-    <row r="324" ht="15.75" customHeight="1"/>
-    <row r="325" ht="15.75" customHeight="1"/>
-    <row r="326" ht="15.75" customHeight="1"/>
-    <row r="327" ht="15.75" customHeight="1"/>
-    <row r="328" ht="15.75" customHeight="1"/>
-    <row r="329" ht="15.75" customHeight="1"/>
-    <row r="330" ht="15.75" customHeight="1"/>
-    <row r="331" ht="15.75" customHeight="1"/>
-    <row r="332" ht="15.75" customHeight="1"/>
-    <row r="333" ht="15.75" customHeight="1"/>
-    <row r="334" ht="15.75" customHeight="1"/>
-    <row r="335" ht="15.75" customHeight="1"/>
-    <row r="336" ht="15.75" customHeight="1"/>
-    <row r="337" ht="15.75" customHeight="1"/>
-    <row r="338" ht="15.75" customHeight="1"/>
-    <row r="339" ht="15.75" customHeight="1"/>
-    <row r="340" ht="15.75" customHeight="1"/>
-    <row r="341" ht="15.75" customHeight="1"/>
-    <row r="342" ht="15.75" customHeight="1"/>
-    <row r="343" ht="15.75" customHeight="1"/>
-    <row r="344" ht="15.75" customHeight="1"/>
-    <row r="345" ht="15.75" customHeight="1"/>
-    <row r="346" ht="15.75" customHeight="1"/>
-    <row r="347" ht="15.75" customHeight="1"/>
-    <row r="348" ht="15.75" customHeight="1"/>
-    <row r="349" ht="15.75" customHeight="1"/>
-    <row r="350" ht="15.75" customHeight="1"/>
-    <row r="351" ht="15.75" customHeight="1"/>
-    <row r="352" ht="15.75" customHeight="1"/>
-    <row r="353" ht="15.75" customHeight="1"/>
-    <row r="354" ht="15.75" customHeight="1"/>
-    <row r="355" ht="15.75" customHeight="1"/>
-    <row r="356" ht="15.75" customHeight="1"/>
-    <row r="357" ht="15.75" customHeight="1"/>
-    <row r="358" ht="15.75" customHeight="1"/>
-    <row r="359" ht="15.75" customHeight="1"/>
-    <row r="360" ht="15.75" customHeight="1"/>
-    <row r="361" ht="15.75" customHeight="1"/>
-    <row r="362" ht="15.75" customHeight="1"/>
-    <row r="363" ht="15.75" customHeight="1"/>
-    <row r="364" ht="15.75" customHeight="1"/>
-    <row r="365" ht="15.75" customHeight="1"/>
-    <row r="366" ht="15.75" customHeight="1"/>
-    <row r="367" ht="15.75" customHeight="1"/>
-    <row r="368" ht="15.75" customHeight="1"/>
-    <row r="369" ht="15.75" customHeight="1"/>
-    <row r="370" ht="15.75" customHeight="1"/>
-    <row r="371" ht="15.75" customHeight="1"/>
-    <row r="372" ht="15.75" customHeight="1"/>
-    <row r="373" ht="15.75" customHeight="1"/>
-    <row r="374" ht="15.75" customHeight="1"/>
-    <row r="375" ht="15.75" customHeight="1"/>
-    <row r="376" ht="15.75" customHeight="1"/>
-    <row r="377" ht="15.75" customHeight="1"/>
-    <row r="378" ht="15.75" customHeight="1"/>
-    <row r="379" ht="15.75" customHeight="1"/>
-    <row r="380" ht="15.75" customHeight="1"/>
-    <row r="381" ht="15.75" customHeight="1"/>
-    <row r="382" ht="15.75" customHeight="1"/>
-    <row r="383" ht="15.75" customHeight="1"/>
-    <row r="384" ht="15.75" customHeight="1"/>
-    <row r="385" ht="15.75" customHeight="1"/>
-    <row r="386" ht="15.75" customHeight="1"/>
-    <row r="387" ht="15.75" customHeight="1"/>
-    <row r="388" ht="15.75" customHeight="1"/>
-    <row r="389" ht="15.75" customHeight="1"/>
-    <row r="390" ht="15.75" customHeight="1"/>
-    <row r="391" ht="15.75" customHeight="1"/>
-    <row r="392" ht="15.75" customHeight="1"/>
-    <row r="393" ht="15.75" customHeight="1"/>
-    <row r="394" ht="15.75" customHeight="1"/>
-    <row r="395" ht="15.75" customHeight="1"/>
-    <row r="396" ht="15.75" customHeight="1"/>
-    <row r="397" ht="15.75" customHeight="1"/>
-    <row r="398" ht="15.75" customHeight="1"/>
-    <row r="399" ht="15.75" customHeight="1"/>
-    <row r="400" ht="15.75" customHeight="1"/>
-    <row r="401" ht="15.75" customHeight="1"/>
-    <row r="402" ht="15.75" customHeight="1"/>
-    <row r="403" ht="15.75" customHeight="1"/>
-    <row r="404" ht="15.75" customHeight="1"/>
-    <row r="405" ht="15.75" customHeight="1"/>
-    <row r="406" ht="15.75" customHeight="1"/>
-    <row r="407" ht="15.75" customHeight="1"/>
-    <row r="408" ht="15.75" customHeight="1"/>
-    <row r="409" ht="15.75" customHeight="1"/>
-    <row r="410" ht="15.75" customHeight="1"/>
-    <row r="411" ht="15.75" customHeight="1"/>
-    <row r="412" ht="15.75" customHeight="1"/>
-    <row r="413" ht="15.75" customHeight="1"/>
-    <row r="414" ht="15.75" customHeight="1"/>
-    <row r="415" ht="15.75" customHeight="1"/>
-    <row r="416" ht="15.75" customHeight="1"/>
-    <row r="417" ht="15.75" customHeight="1"/>
-    <row r="418" ht="15.75" customHeight="1"/>
-    <row r="419" ht="15.75" customHeight="1"/>
-    <row r="420" ht="15.75" customHeight="1"/>
-    <row r="421" ht="15.75" customHeight="1"/>
-    <row r="422" ht="15.75" customHeight="1"/>
-    <row r="423" ht="15.75" customHeight="1"/>
-    <row r="424" ht="15.75" customHeight="1"/>
-    <row r="425" ht="15.75" customHeight="1"/>
-    <row r="426" ht="15.75" customHeight="1"/>
-    <row r="427" ht="15.75" customHeight="1"/>
-    <row r="428" ht="15.75" customHeight="1"/>
-    <row r="429" ht="15.75" customHeight="1"/>
-    <row r="430" ht="15.75" customHeight="1"/>
-    <row r="431" ht="15.75" customHeight="1"/>
-    <row r="432" ht="15.75" customHeight="1"/>
-    <row r="433" ht="15.75" customHeight="1"/>
-    <row r="434" ht="15.75" customHeight="1"/>
-    <row r="435" ht="15.75" customHeight="1"/>
-    <row r="436" ht="15.75" customHeight="1"/>
-    <row r="437" ht="15.75" customHeight="1"/>
-    <row r="438" ht="15.75" customHeight="1"/>
-    <row r="439" ht="15.75" customHeight="1"/>
-    <row r="440" ht="15.75" customHeight="1"/>
-    <row r="441" ht="15.75" customHeight="1"/>
-    <row r="442" ht="15.75" customHeight="1"/>
-    <row r="443" ht="15.75" customHeight="1"/>
-    <row r="444" ht="15.75" customHeight="1"/>
-    <row r="445" ht="15.75" customHeight="1"/>
-    <row r="446" ht="15.75" customHeight="1"/>
-    <row r="447" ht="15.75" customHeight="1"/>
-    <row r="448" ht="15.75" customHeight="1"/>
-    <row r="449" ht="15.75" customHeight="1"/>
-    <row r="450" ht="15.75" customHeight="1"/>
-    <row r="451" ht="15.75" customHeight="1"/>
-    <row r="452" ht="15.75" customHeight="1"/>
-    <row r="453" ht="15.75" customHeight="1"/>
-    <row r="454" ht="15.75" customHeight="1"/>
-    <row r="455" ht="15.75" customHeight="1"/>
-    <row r="456" ht="15.75" customHeight="1"/>
-    <row r="457" ht="15.75" customHeight="1"/>
-    <row r="458" ht="15.75" customHeight="1"/>
-    <row r="459" ht="15.75" customHeight="1"/>
-    <row r="460" ht="15.75" customHeight="1"/>
-    <row r="461" ht="15.75" customHeight="1"/>
-    <row r="462" ht="15.75" customHeight="1"/>
-    <row r="463" ht="15.75" customHeight="1"/>
-    <row r="464" ht="15.75" customHeight="1"/>
-    <row r="465" ht="15.75" customHeight="1"/>
-    <row r="466" ht="15.75" customHeight="1"/>
-    <row r="467" ht="15.75" customHeight="1"/>
-    <row r="468" ht="15.75" customHeight="1"/>
-    <row r="469" ht="15.75" customHeight="1"/>
-    <row r="470" ht="15.75" customHeight="1"/>
-    <row r="471" ht="15.75" customHeight="1"/>
-    <row r="472" ht="15.75" customHeight="1"/>
-    <row r="473" ht="15.75" customHeight="1"/>
-    <row r="474" ht="15.75" customHeight="1"/>
-    <row r="475" ht="15.75" customHeight="1"/>
-    <row r="476" ht="15.75" customHeight="1"/>
-    <row r="477" ht="15.75" customHeight="1"/>
-    <row r="478" ht="15.75" customHeight="1"/>
-    <row r="479" ht="15.75" customHeight="1"/>
-    <row r="480" ht="15.75" customHeight="1"/>
-    <row r="481" ht="15.75" customHeight="1"/>
-    <row r="482" ht="15.75" customHeight="1"/>
-    <row r="483" ht="15.75" customHeight="1"/>
-    <row r="484" ht="15.75" customHeight="1"/>
-    <row r="485" ht="15.75" customHeight="1"/>
-    <row r="486" ht="15.75" customHeight="1"/>
-    <row r="487" ht="15.75" customHeight="1"/>
-    <row r="488" ht="15.75" customHeight="1"/>
-    <row r="489" ht="15.75" customHeight="1"/>
-    <row r="490" ht="15.75" customHeight="1"/>
-    <row r="491" ht="15.75" customHeight="1"/>
-    <row r="492" ht="15.75" customHeight="1"/>
-    <row r="493" ht="15.75" customHeight="1"/>
-    <row r="494" ht="15.75" customHeight="1"/>
-    <row r="495" ht="15.75" customHeight="1"/>
-    <row r="496" ht="15.75" customHeight="1"/>
-    <row r="497" ht="15.75" customHeight="1"/>
-    <row r="498" ht="15.75" customHeight="1"/>
-    <row r="499" ht="15.75" customHeight="1"/>
-    <row r="500" ht="15.75" customHeight="1"/>
-    <row r="501" ht="15.75" customHeight="1"/>
-    <row r="502" ht="15.75" customHeight="1"/>
-    <row r="503" ht="15.75" customHeight="1"/>
-    <row r="504" ht="15.75" customHeight="1"/>
-    <row r="505" ht="15.75" customHeight="1"/>
-    <row r="506" ht="15.75" customHeight="1"/>
-    <row r="507" ht="15.75" customHeight="1"/>
-    <row r="508" ht="15.75" customHeight="1"/>
-    <row r="509" ht="15.75" customHeight="1"/>
-    <row r="510" ht="15.75" customHeight="1"/>
-    <row r="511" ht="15.75" customHeight="1"/>
-    <row r="512" ht="15.75" customHeight="1"/>
-    <row r="513" ht="15.75" customHeight="1"/>
-    <row r="514" ht="15.75" customHeight="1"/>
-    <row r="515" ht="15.75" customHeight="1"/>
-    <row r="516" ht="15.75" customHeight="1"/>
-    <row r="517" ht="15.75" customHeight="1"/>
-    <row r="518" ht="15.75" customHeight="1"/>
-    <row r="519" ht="15.75" customHeight="1"/>
-    <row r="520" ht="15.75" customHeight="1"/>
-    <row r="521" ht="15.75" customHeight="1"/>
-    <row r="522" ht="15.75" customHeight="1"/>
-    <row r="523" ht="15.75" customHeight="1"/>
-    <row r="524" ht="15.75" customHeight="1"/>
-    <row r="525" ht="15.75" customHeight="1"/>
-    <row r="526" ht="15.75" customHeight="1"/>
-    <row r="527" ht="15.75" customHeight="1"/>
-    <row r="528" ht="15.75" customHeight="1"/>
-    <row r="529" ht="15.75" customHeight="1"/>
-    <row r="530" ht="15.75" customHeight="1"/>
-    <row r="531" ht="15.75" customHeight="1"/>
-    <row r="532" ht="15.75" customHeight="1"/>
-    <row r="533" ht="15.75" customHeight="1"/>
-    <row r="534" ht="15.75" customHeight="1"/>
-    <row r="535" ht="15.75" customHeight="1"/>
-    <row r="536" ht="15.75" customHeight="1"/>
-    <row r="537" ht="15.75" customHeight="1"/>
-    <row r="538" ht="15.75" customHeight="1"/>
-    <row r="539" ht="15.75" customHeight="1"/>
-    <row r="540" ht="15.75" customHeight="1"/>
-    <row r="541" ht="15.75" customHeight="1"/>
-    <row r="542" ht="15.75" customHeight="1"/>
-    <row r="543" ht="15.75" customHeight="1"/>
-    <row r="544" ht="15.75" customHeight="1"/>
-    <row r="545" ht="15.75" customHeight="1"/>
-    <row r="546" ht="15.75" customHeight="1"/>
-    <row r="547" ht="15.75" customHeight="1"/>
-    <row r="548" ht="15.75" customHeight="1"/>
-    <row r="549" ht="15.75" customHeight="1"/>
-    <row r="550" ht="15.75" customHeight="1"/>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
-    <row r="583" ht="15.75" customHeight="1"/>
-    <row r="584" ht="15.75" customHeight="1"/>
-    <row r="585" ht="15.75" customHeight="1"/>
-    <row r="586" ht="15.75" customHeight="1"/>
-    <row r="587" ht="15.75" customHeight="1"/>
-    <row r="588" ht="15.75" customHeight="1"/>
-    <row r="589" ht="15.75" customHeight="1"/>
-    <row r="590" ht="15.75" customHeight="1"/>
-    <row r="591" ht="15.75" customHeight="1"/>
-    <row r="592" ht="15.75" customHeight="1"/>
-    <row r="593" ht="15.75" customHeight="1"/>
-    <row r="594" ht="15.75" customHeight="1"/>
-    <row r="595" ht="15.75" customHeight="1"/>
-    <row r="596" ht="15.75" customHeight="1"/>
-    <row r="597" ht="15.75" customHeight="1"/>
-    <row r="598" ht="15.75" customHeight="1"/>
-    <row r="599" ht="15.75" customHeight="1"/>
-    <row r="600" ht="15.75" customHeight="1"/>
-    <row r="601" ht="15.75" customHeight="1"/>
-    <row r="602" ht="15.75" customHeight="1"/>
-    <row r="603" ht="15.75" customHeight="1"/>
-    <row r="604" ht="15.75" customHeight="1"/>
-    <row r="605" ht="15.75" customHeight="1"/>
-    <row r="606" ht="15.75" customHeight="1"/>
-    <row r="607" ht="15.75" customHeight="1"/>
-    <row r="608" ht="15.75" customHeight="1"/>
-    <row r="609" ht="15.75" customHeight="1"/>
-    <row r="610" ht="15.75" customHeight="1"/>
-    <row r="611" ht="15.75" customHeight="1"/>
-    <row r="612" ht="15.75" customHeight="1"/>
-    <row r="613" ht="15.75" customHeight="1"/>
-    <row r="614" ht="15.75" customHeight="1"/>
-    <row r="615" ht="15.75" customHeight="1"/>
-    <row r="616" ht="15.75" customHeight="1"/>
-    <row r="617" ht="15.75" customHeight="1"/>
-    <row r="618" ht="15.75" customHeight="1"/>
-    <row r="619" ht="15.75" customHeight="1"/>
-    <row r="620" ht="15.75" customHeight="1"/>
-    <row r="621" ht="15.75" customHeight="1"/>
-    <row r="622" ht="15.75" customHeight="1"/>
-    <row r="623" ht="15.75" customHeight="1"/>
-    <row r="624" ht="15.75" customHeight="1"/>
-    <row r="625" ht="15.75" customHeight="1"/>
-    <row r="626" ht="15.75" customHeight="1"/>
-    <row r="627" ht="15.75" customHeight="1"/>
-    <row r="628" ht="15.75" customHeight="1"/>
-    <row r="629" ht="15.75" customHeight="1"/>
-    <row r="630" ht="15.75" customHeight="1"/>
-    <row r="631" ht="15.75" customHeight="1"/>
-    <row r="632" ht="15.75" customHeight="1"/>
-    <row r="633" ht="15.75" customHeight="1"/>
-    <row r="634" ht="15.75" customHeight="1"/>
-    <row r="635" ht="15.75" customHeight="1"/>
-    <row r="636" ht="15.75" customHeight="1"/>
-    <row r="637" ht="15.75" customHeight="1"/>
-    <row r="638" ht="15.75" customHeight="1"/>
-    <row r="639" ht="15.75" customHeight="1"/>
-    <row r="640" ht="15.75" customHeight="1"/>
-    <row r="641" ht="15.75" customHeight="1"/>
-    <row r="642" ht="15.75" customHeight="1"/>
-    <row r="643" ht="15.75" customHeight="1"/>
-    <row r="644" ht="15.75" customHeight="1"/>
-    <row r="645" ht="15.75" customHeight="1"/>
-    <row r="646" ht="15.75" customHeight="1"/>
-    <row r="647" ht="15.75" customHeight="1"/>
-    <row r="648" ht="15.75" customHeight="1"/>
-    <row r="649" ht="15.75" customHeight="1"/>
-    <row r="650" ht="15.75" customHeight="1"/>
-    <row r="651" ht="15.75" customHeight="1"/>
-    <row r="652" ht="15.75" customHeight="1"/>
-    <row r="653" ht="15.75" customHeight="1"/>
-    <row r="654" ht="15.75" customHeight="1"/>
-    <row r="655" ht="15.75" customHeight="1"/>
-    <row r="656" ht="15.75" customHeight="1"/>
-    <row r="657" ht="15.75" customHeight="1"/>
-    <row r="658" ht="15.75" customHeight="1"/>
-    <row r="659" ht="15.75" customHeight="1"/>
-    <row r="660" ht="15.75" customHeight="1"/>
-    <row r="661" ht="15.75" customHeight="1"/>
-    <row r="662" ht="15.75" customHeight="1"/>
-    <row r="663" ht="15.75" customHeight="1"/>
-    <row r="664" ht="15.75" customHeight="1"/>
-    <row r="665" ht="15.75" customHeight="1"/>
-    <row r="666" ht="15.75" customHeight="1"/>
-    <row r="667" ht="15.75" customHeight="1"/>
-    <row r="668" ht="15.75" customHeight="1"/>
-    <row r="669" ht="15.75" customHeight="1"/>
-    <row r="670" ht="15.75" customHeight="1"/>
-    <row r="671" ht="15.75" customHeight="1"/>
-    <row r="672" ht="15.75" customHeight="1"/>
-    <row r="673" ht="15.75" customHeight="1"/>
-    <row r="674" ht="15.75" customHeight="1"/>
-    <row r="675" ht="15.75" customHeight="1"/>
-    <row r="676" ht="15.75" customHeight="1"/>
-    <row r="677" ht="15.75" customHeight="1"/>
-    <row r="678" ht="15.75" customHeight="1"/>
-    <row r="679" ht="15.75" customHeight="1"/>
-    <row r="680" ht="15.75" customHeight="1"/>
-    <row r="681" ht="15.75" customHeight="1"/>
-    <row r="682" ht="15.75" customHeight="1"/>
-    <row r="683" ht="15.75" customHeight="1"/>
-    <row r="684" ht="15.75" customHeight="1"/>
-    <row r="685" ht="15.75" customHeight="1"/>
-    <row r="686" ht="15.75" customHeight="1"/>
-    <row r="687" ht="15.75" customHeight="1"/>
-    <row r="688" ht="15.75" customHeight="1"/>
-    <row r="689" ht="15.75" customHeight="1"/>
-    <row r="690" ht="15.75" customHeight="1"/>
-    <row r="691" ht="15.75" customHeight="1"/>
-    <row r="692" ht="15.75" customHeight="1"/>
-    <row r="693" ht="15.75" customHeight="1"/>
-    <row r="694" ht="15.75" customHeight="1"/>
-    <row r="695" ht="15.75" customHeight="1"/>
-    <row r="696" ht="15.75" customHeight="1"/>
-    <row r="697" ht="15.75" customHeight="1"/>
-    <row r="698" ht="15.75" customHeight="1"/>
-    <row r="699" ht="15.75" customHeight="1"/>
-    <row r="700" ht="15.75" customHeight="1"/>
-    <row r="701" ht="15.75" customHeight="1"/>
-    <row r="702" ht="15.75" customHeight="1"/>
-    <row r="703" ht="15.75" customHeight="1"/>
-    <row r="704" ht="15.75" customHeight="1"/>
-    <row r="705" ht="15.75" customHeight="1"/>
-    <row r="706" ht="15.75" customHeight="1"/>
-    <row r="707" ht="15.75" customHeight="1"/>
-    <row r="708" ht="15.75" customHeight="1"/>
-    <row r="709" ht="15.75" customHeight="1"/>
-    <row r="710" ht="15.75" customHeight="1"/>
-    <row r="711" ht="15.75" customHeight="1"/>
-    <row r="712" ht="15.75" customHeight="1"/>
-    <row r="713" ht="15.75" customHeight="1"/>
-    <row r="714" ht="15.75" customHeight="1"/>
-    <row r="715" ht="15.75" customHeight="1"/>
-    <row r="716" ht="15.75" customHeight="1"/>
-    <row r="717" ht="15.75" customHeight="1"/>
-    <row r="718" ht="15.75" customHeight="1"/>
-    <row r="719" ht="15.75" customHeight="1"/>
-    <row r="720" ht="15.75" customHeight="1"/>
-    <row r="721" ht="15.75" customHeight="1"/>
-    <row r="722" ht="15.75" customHeight="1"/>
-    <row r="723" ht="15.75" customHeight="1"/>
-    <row r="724" ht="15.75" customHeight="1"/>
-    <row r="725" ht="15.75" customHeight="1"/>
-    <row r="726" ht="15.75" customHeight="1"/>
-    <row r="727" ht="15.75" customHeight="1"/>
-    <row r="728" ht="15.75" customHeight="1"/>
-    <row r="729" ht="15.75" customHeight="1"/>
-    <row r="730" ht="15.75" customHeight="1"/>
-    <row r="731" ht="15.75" customHeight="1"/>
-    <row r="732" ht="15.75" customHeight="1"/>
-    <row r="733" ht="15.75" customHeight="1"/>
-    <row r="734" ht="15.75" customHeight="1"/>
-    <row r="735" ht="15.75" customHeight="1"/>
-    <row r="736" ht="15.75" customHeight="1"/>
-    <row r="737" ht="15.75" customHeight="1"/>
-    <row r="738" ht="15.75" customHeight="1"/>
-    <row r="739" ht="15.75" customHeight="1"/>
-    <row r="740" ht="15.75" customHeight="1"/>
-    <row r="741" ht="15.75" customHeight="1"/>
-    <row r="742" ht="15.75" customHeight="1"/>
-    <row r="743" ht="15.75" customHeight="1"/>
-    <row r="744" ht="15.75" customHeight="1"/>
-    <row r="745" ht="15.75" customHeight="1"/>
-    <row r="746" ht="15.75" customHeight="1"/>
-    <row r="747" ht="15.75" customHeight="1"/>
-    <row r="748" ht="15.75" customHeight="1"/>
-    <row r="749" ht="15.75" customHeight="1"/>
-    <row r="750" ht="15.75" customHeight="1"/>
-    <row r="751" ht="15.75" customHeight="1"/>
-    <row r="752" ht="15.75" customHeight="1"/>
-    <row r="753" ht="15.75" customHeight="1"/>
-    <row r="754" ht="15.75" customHeight="1"/>
-    <row r="755" ht="15.75" customHeight="1"/>
-    <row r="756" ht="15.75" customHeight="1"/>
-    <row r="757" ht="15.75" customHeight="1"/>
-    <row r="758" ht="15.75" customHeight="1"/>
-    <row r="759" ht="15.75" customHeight="1"/>
-    <row r="760" ht="15.75" customHeight="1"/>
-    <row r="761" ht="15.75" customHeight="1"/>
-    <row r="762" ht="15.75" customHeight="1"/>
-    <row r="763" ht="15.75" customHeight="1"/>
-    <row r="764" ht="15.75" customHeight="1"/>
-    <row r="765" ht="15.75" customHeight="1"/>
-    <row r="766" ht="15.75" customHeight="1"/>
-    <row r="767" ht="15.75" customHeight="1"/>
-    <row r="768" ht="15.75" customHeight="1"/>
-    <row r="769" ht="15.75" customHeight="1"/>
-    <row r="770" ht="15.75" customHeight="1"/>
-    <row r="771" ht="15.75" customHeight="1"/>
-    <row r="772" ht="15.75" customHeight="1"/>
-    <row r="773" ht="15.75" customHeight="1"/>
-    <row r="774" ht="15.75" customHeight="1"/>
-    <row r="775" ht="15.75" customHeight="1"/>
-    <row r="776" ht="15.75" customHeight="1"/>
-    <row r="777" ht="15.75" customHeight="1"/>
-    <row r="778" ht="15.75" customHeight="1"/>
-    <row r="779" ht="15.75" customHeight="1"/>
-    <row r="780" ht="15.75" customHeight="1"/>
-    <row r="781" ht="15.75" customHeight="1"/>
-    <row r="782" ht="15.75" customHeight="1"/>
-    <row r="783" ht="15.75" customHeight="1"/>
-    <row r="784" ht="15.75" customHeight="1"/>
-    <row r="785" ht="15.75" customHeight="1"/>
-    <row r="786" ht="15.75" customHeight="1"/>
-    <row r="787" ht="15.75" customHeight="1"/>
-    <row r="788" ht="15.75" customHeight="1"/>
-    <row r="789" ht="15.75" customHeight="1"/>
-    <row r="790" ht="15.75" customHeight="1"/>
-    <row r="791" ht="15.75" customHeight="1"/>
-    <row r="792" ht="15.75" customHeight="1"/>
-    <row r="793" ht="15.75" customHeight="1"/>
-    <row r="794" ht="15.75" customHeight="1"/>
-    <row r="795" ht="15.75" customHeight="1"/>
-    <row r="796" ht="15.75" customHeight="1"/>
-    <row r="797" ht="15.75" customHeight="1"/>
-    <row r="798" ht="15.75" customHeight="1"/>
-    <row r="799" ht="15.75" customHeight="1"/>
-    <row r="800" ht="15.75" customHeight="1"/>
-    <row r="801" ht="15.75" customHeight="1"/>
-    <row r="802" ht="15.75" customHeight="1"/>
-    <row r="803" ht="15.75" customHeight="1"/>
-    <row r="804" ht="15.75" customHeight="1"/>
-    <row r="805" ht="15.75" customHeight="1"/>
-    <row r="806" ht="15.75" customHeight="1"/>
-    <row r="807" ht="15.75" customHeight="1"/>
-    <row r="808" ht="15.75" customHeight="1"/>
-    <row r="809" ht="15.75" customHeight="1"/>
-    <row r="810" ht="15.75" customHeight="1"/>
-    <row r="811" ht="15.75" customHeight="1"/>
-    <row r="812" ht="15.75" customHeight="1"/>
-    <row r="813" ht="15.75" customHeight="1"/>
-    <row r="814" ht="15.75" customHeight="1"/>
-    <row r="815" ht="15.75" customHeight="1"/>
-    <row r="816" ht="15.75" customHeight="1"/>
-    <row r="817" ht="15.75" customHeight="1"/>
-    <row r="818" ht="15.75" customHeight="1"/>
-    <row r="819" ht="15.75" customHeight="1"/>
-    <row r="820" ht="15.75" customHeight="1"/>
-    <row r="821" ht="15.75" customHeight="1"/>
-    <row r="822" ht="15.75" customHeight="1"/>
-    <row r="823" ht="15.75" customHeight="1"/>
-    <row r="824" ht="15.75" customHeight="1"/>
-    <row r="825" ht="15.75" customHeight="1"/>
-    <row r="826" ht="15.75" customHeight="1"/>
-    <row r="827" ht="15.75" customHeight="1"/>
-    <row r="828" ht="15.75" customHeight="1"/>
-    <row r="829" ht="15.75" customHeight="1"/>
-    <row r="830" ht="15.75" customHeight="1"/>
-    <row r="831" ht="15.75" customHeight="1"/>
-    <row r="832" ht="15.75" customHeight="1"/>
-    <row r="833" ht="15.75" customHeight="1"/>
-    <row r="834" ht="15.75" customHeight="1"/>
-    <row r="835" ht="15.75" customHeight="1"/>
-    <row r="836" ht="15.75" customHeight="1"/>
-    <row r="837" ht="15.75" customHeight="1"/>
-    <row r="838" ht="15.75" customHeight="1"/>
-    <row r="839" ht="15.75" customHeight="1"/>
-    <row r="840" ht="15.75" customHeight="1"/>
-    <row r="841" ht="15.75" customHeight="1"/>
-    <row r="842" ht="15.75" customHeight="1"/>
-    <row r="843" ht="15.75" customHeight="1"/>
-    <row r="844" ht="15.75" customHeight="1"/>
-    <row r="845" ht="15.75" customHeight="1"/>
-    <row r="846" ht="15.75" customHeight="1"/>
-    <row r="847" ht="15.75" customHeight="1"/>
-    <row r="848" ht="15.75" customHeight="1"/>
-    <row r="849" ht="15.75" customHeight="1"/>
-    <row r="850" ht="15.75" customHeight="1"/>
-    <row r="851" ht="15.75" customHeight="1"/>
-    <row r="852" ht="15.75" customHeight="1"/>
-    <row r="853" ht="15.75" customHeight="1"/>
-    <row r="854" ht="15.75" customHeight="1"/>
-    <row r="855" ht="15.75" customHeight="1"/>
-    <row r="856" ht="15.75" customHeight="1"/>
-    <row r="857" ht="15.75" customHeight="1"/>
-    <row r="858" ht="15.75" customHeight="1"/>
-    <row r="859" ht="15.75" customHeight="1"/>
-    <row r="860" ht="15.75" customHeight="1"/>
-    <row r="861" ht="15.75" customHeight="1"/>
-    <row r="862" ht="15.75" customHeight="1"/>
-    <row r="863" ht="15.75" customHeight="1"/>
-    <row r="864" ht="15.75" customHeight="1"/>
-    <row r="865" ht="15.75" customHeight="1"/>
-    <row r="866" ht="15.75" customHeight="1"/>
-    <row r="867" ht="15.75" customHeight="1"/>
-    <row r="868" ht="15.75" customHeight="1"/>
-    <row r="869" ht="15.75" customHeight="1"/>
-    <row r="870" ht="15.75" customHeight="1"/>
-    <row r="871" ht="15.75" customHeight="1"/>
-    <row r="872" ht="15.75" customHeight="1"/>
-    <row r="873" ht="15.75" customHeight="1"/>
-    <row r="874" ht="15.75" customHeight="1"/>
-    <row r="875" ht="15.75" customHeight="1"/>
-    <row r="876" ht="15.75" customHeight="1"/>
-    <row r="877" ht="15.75" customHeight="1"/>
-    <row r="878" ht="15.75" customHeight="1"/>
-    <row r="879" ht="15.75" customHeight="1"/>
-    <row r="880" ht="15.75" customHeight="1"/>
-    <row r="881" ht="15.75" customHeight="1"/>
-    <row r="882" ht="15.75" customHeight="1"/>
-    <row r="883" ht="15.75" customHeight="1"/>
-    <row r="884" ht="15.75" customHeight="1"/>
-    <row r="885" ht="15.75" customHeight="1"/>
-    <row r="886" ht="15.75" customHeight="1"/>
-    <row r="887" ht="15.75" customHeight="1"/>
-    <row r="888" ht="15.75" customHeight="1"/>
-    <row r="889" ht="15.75" customHeight="1"/>
-    <row r="890" ht="15.75" customHeight="1"/>
-    <row r="891" ht="15.75" customHeight="1"/>
-    <row r="892" ht="15.75" customHeight="1"/>
-    <row r="893" ht="15.75" customHeight="1"/>
-    <row r="894" ht="15.75" customHeight="1"/>
-    <row r="895" ht="15.75" customHeight="1"/>
-    <row r="896" ht="15.75" customHeight="1"/>
-    <row r="897" ht="15.75" customHeight="1"/>
-    <row r="898" ht="15.75" customHeight="1"/>
-    <row r="899" ht="15.75" customHeight="1"/>
-    <row r="900" ht="15.75" customHeight="1"/>
-    <row r="901" ht="15.75" customHeight="1"/>
-    <row r="902" ht="15.75" customHeight="1"/>
-    <row r="903" ht="15.75" customHeight="1"/>
-    <row r="904" ht="15.75" customHeight="1"/>
-    <row r="905" ht="15.75" customHeight="1"/>
-    <row r="906" ht="15.75" customHeight="1"/>
-    <row r="907" ht="15.75" customHeight="1"/>
-    <row r="908" ht="15.75" customHeight="1"/>
-    <row r="909" ht="15.75" customHeight="1"/>
-    <row r="910" ht="15.75" customHeight="1"/>
-    <row r="911" ht="15.75" customHeight="1"/>
-    <row r="912" ht="15.75" customHeight="1"/>
-    <row r="913" ht="15.75" customHeight="1"/>
-    <row r="914" ht="15.75" customHeight="1"/>
-    <row r="915" ht="15.75" customHeight="1"/>
-    <row r="916" ht="15.75" customHeight="1"/>
-    <row r="917" ht="15.75" customHeight="1"/>
-    <row r="918" ht="15.75" customHeight="1"/>
-    <row r="919" ht="15.75" customHeight="1"/>
-    <row r="920" ht="15.75" customHeight="1"/>
-    <row r="921" ht="15.75" customHeight="1"/>
-    <row r="922" ht="15.75" customHeight="1"/>
-    <row r="923" ht="15.75" customHeight="1"/>
-    <row r="924" ht="15.75" customHeight="1"/>
-    <row r="925" ht="15.75" customHeight="1"/>
-    <row r="926" ht="15.75" customHeight="1"/>
-    <row r="927" ht="15.75" customHeight="1"/>
-    <row r="928" ht="15.75" customHeight="1"/>
-    <row r="929" ht="15.75" customHeight="1"/>
-    <row r="930" ht="15.75" customHeight="1"/>
-    <row r="931" ht="15.75" customHeight="1"/>
-    <row r="932" ht="15.75" customHeight="1"/>
-    <row r="933" ht="15.75" customHeight="1"/>
-    <row r="934" ht="15.75" customHeight="1"/>
-    <row r="935" ht="15.75" customHeight="1"/>
-    <row r="936" ht="15.75" customHeight="1"/>
-    <row r="937" ht="15.75" customHeight="1"/>
-    <row r="938" ht="15.75" customHeight="1"/>
-    <row r="939" ht="15.75" customHeight="1"/>
-    <row r="940" ht="15.75" customHeight="1"/>
-    <row r="941" ht="15.75" customHeight="1"/>
-    <row r="942" ht="15.75" customHeight="1"/>
-    <row r="943" ht="15.75" customHeight="1"/>
-    <row r="944" ht="15.75" customHeight="1"/>
-    <row r="945" ht="15.75" customHeight="1"/>
-    <row r="946" ht="15.75" customHeight="1"/>
-    <row r="947" ht="15.75" customHeight="1"/>
-    <row r="948" ht="15.75" customHeight="1"/>
-    <row r="949" ht="15.75" customHeight="1"/>
-    <row r="950" ht="15.75" customHeight="1"/>
-    <row r="951" ht="15.75" customHeight="1"/>
-    <row r="952" ht="15.75" customHeight="1"/>
-    <row r="953" ht="15.75" customHeight="1"/>
-    <row r="954" ht="15.75" customHeight="1"/>
-    <row r="955" ht="15.75" customHeight="1"/>
-    <row r="956" ht="15.75" customHeight="1"/>
-    <row r="957" ht="15.75" customHeight="1"/>
-    <row r="958" ht="15.75" customHeight="1"/>
-    <row r="959" ht="15.75" customHeight="1"/>
-    <row r="960" ht="15.75" customHeight="1"/>
-    <row r="961" ht="15.75" customHeight="1"/>
-    <row r="962" ht="15.75" customHeight="1"/>
-    <row r="963" ht="15.75" customHeight="1"/>
-    <row r="964" ht="15.75" customHeight="1"/>
-    <row r="965" ht="15.75" customHeight="1"/>
-    <row r="966" ht="15.75" customHeight="1"/>
-    <row r="967" ht="15.75" customHeight="1"/>
-    <row r="968" ht="15.75" customHeight="1"/>
-    <row r="969" ht="15.75" customHeight="1"/>
-    <row r="970" ht="15.75" customHeight="1"/>
-    <row r="971" ht="15.75" customHeight="1"/>
-    <row r="972" ht="15.75" customHeight="1"/>
-    <row r="973" ht="15.75" customHeight="1"/>
-    <row r="974" ht="15.75" customHeight="1"/>
-    <row r="975" ht="15.75" customHeight="1"/>
-    <row r="976" ht="15.75" customHeight="1"/>
-    <row r="977" ht="15.75" customHeight="1"/>
-    <row r="978" ht="15.75" customHeight="1"/>
-    <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
-    <row r="985" ht="15.75" customHeight="1"/>
-    <row r="986" ht="15.75" customHeight="1"/>
-    <row r="987" ht="15.75" customHeight="1"/>
-    <row r="988" ht="15.75" customHeight="1"/>
-    <row r="989" ht="15.75" customHeight="1"/>
-    <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="17.14"/>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="13.57"/>
-    <col customWidth="1" min="4" max="4" width="16.29"/>
-    <col customWidth="1" min="5" max="5" width="17.43"/>
-    <col customWidth="1" min="6" max="6" width="5.29"/>
-    <col customWidth="1" min="7" max="7" width="11.14"/>
-    <col customWidth="1" min="8" max="8" width="12.14"/>
-    <col customWidth="1" min="9" max="9" width="11.43"/>
-    <col customWidth="1" min="10" max="10" width="11.71"/>
-    <col customWidth="1" min="11" max="11" width="15.57"/>
-    <col customWidth="1" min="12" max="13" width="5.86"/>
-    <col customWidth="1" min="14" max="14" width="3.86"/>
-    <col customWidth="1" min="15" max="15" width="5.57"/>
-    <col customWidth="1" min="16" max="16" width="10.71"/>
-    <col customWidth="1" min="17" max="17" width="5.0"/>
-    <col customWidth="1" min="18" max="18" width="12.0"/>
-    <col customWidth="1" min="19" max="19" width="9.43"/>
-    <col customWidth="1" min="20" max="20" width="4.43"/>
-    <col customWidth="1" min="21" max="21" width="12.29"/>
-    <col customWidth="1" min="22" max="22" width="13.0"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="23">
-        <f t="shared" ref="A2:A9" si="1">TODAY()</f>
-        <v>43292</v>
-      </c>
-      <c r="B2" s="23">
-        <f t="shared" ref="B2:B9" si="2">A2 + 365</f>
-        <v>43657</v>
-      </c>
-      <c r="E2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="24">
-        <v>18.75</v>
-      </c>
-      <c r="M2" s="24">
-        <v>9.375</v>
-      </c>
-      <c r="N2">
-        <v>0.0</v>
-      </c>
-      <c r="O2">
-        <v>0.0</v>
-      </c>
-      <c r="P2">
-        <v>0.0</v>
-      </c>
-      <c r="Q2">
-        <v>0.0</v>
-      </c>
-      <c r="R2">
-        <v>0.0</v>
-      </c>
-      <c r="S2" s="24">
-        <v>18.75</v>
-      </c>
-      <c r="T2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="23">
-        <f t="shared" si="1"/>
-        <v>43292</v>
-      </c>
-      <c r="B3" s="23">
-        <f t="shared" si="2"/>
-        <v>43657</v>
-      </c>
-      <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3">
-        <v>0.0</v>
-      </c>
-      <c r="M3">
-        <v>0.0</v>
-      </c>
-      <c r="N3">
-        <v>0.0</v>
-      </c>
-      <c r="O3">
-        <v>0.0</v>
-      </c>
-      <c r="P3" s="24">
-        <v>31.25</v>
-      </c>
-      <c r="Q3">
-        <v>0.0</v>
-      </c>
-      <c r="R3">
-        <v>0.0</v>
-      </c>
-      <c r="S3">
-        <v>0.0</v>
-      </c>
-      <c r="T3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="23">
-        <f t="shared" si="1"/>
-        <v>43292</v>
-      </c>
-      <c r="B4" s="23">
-        <f t="shared" si="2"/>
-        <v>43657</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H4" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" s="24">
-        <v>0.0</v>
-      </c>
-      <c r="M4">
-        <v>0.0</v>
-      </c>
-      <c r="N4">
-        <v>0.0</v>
-      </c>
-      <c r="O4">
-        <v>0.0</v>
-      </c>
-      <c r="P4" s="24">
-        <v>31.25</v>
-      </c>
-      <c r="Q4">
-        <v>0.0</v>
-      </c>
-      <c r="R4">
-        <v>0.0</v>
-      </c>
-      <c r="S4" s="24">
-        <v>0.0</v>
-      </c>
-      <c r="T4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="23">
-        <f t="shared" si="1"/>
-        <v>43292</v>
-      </c>
-      <c r="B5" s="23">
-        <f t="shared" si="2"/>
-        <v>43657</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="24">
-        <v>20.75</v>
-      </c>
-      <c r="M5">
-        <v>0.0</v>
-      </c>
-      <c r="N5">
-        <v>0.0</v>
-      </c>
-      <c r="O5">
-        <v>0.0</v>
-      </c>
-      <c r="P5">
-        <v>0.0</v>
-      </c>
-      <c r="Q5">
-        <v>0.0</v>
-      </c>
-      <c r="R5">
-        <v>0.0</v>
-      </c>
-      <c r="S5" s="24">
-        <v>20.75</v>
-      </c>
-      <c r="T5">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="23">
-        <f t="shared" si="1"/>
-        <v>43292</v>
-      </c>
-      <c r="B6" s="23">
-        <f t="shared" si="2"/>
-        <v>43657</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="24">
-        <v>18.75</v>
-      </c>
-      <c r="M6" s="24">
-        <v>9.375</v>
-      </c>
-      <c r="N6">
-        <v>0.0</v>
-      </c>
-      <c r="O6">
-        <v>0.0</v>
-      </c>
-      <c r="P6">
-        <v>0.0</v>
-      </c>
-      <c r="Q6">
-        <v>0.0</v>
-      </c>
-      <c r="R6">
-        <v>0.0</v>
-      </c>
-      <c r="S6" s="24">
-        <v>18.75</v>
-      </c>
-      <c r="T6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="23">
-        <f t="shared" si="1"/>
-        <v>43292</v>
-      </c>
-      <c r="B7" s="23">
-        <f t="shared" si="2"/>
-        <v>43657</v>
-      </c>
-      <c r="E7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7">
-        <v>0.0</v>
-      </c>
-      <c r="M7">
-        <v>0.0</v>
-      </c>
-      <c r="N7">
-        <v>0.0</v>
-      </c>
-      <c r="O7">
-        <v>0.0</v>
-      </c>
-      <c r="P7" s="24">
-        <v>31.25</v>
-      </c>
-      <c r="Q7">
-        <v>0.0</v>
-      </c>
-      <c r="R7">
-        <v>0.0</v>
-      </c>
-      <c r="S7">
-        <v>0.0</v>
-      </c>
-      <c r="T7">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="23">
-        <f t="shared" si="1"/>
-        <v>43292</v>
-      </c>
-      <c r="B8" s="23">
-        <f t="shared" si="2"/>
-        <v>43657</v>
-      </c>
-      <c r="E8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" t="s">
-        <v>68</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="24">
-        <v>0.0</v>
-      </c>
-      <c r="M8">
-        <v>0.0</v>
-      </c>
-      <c r="N8">
-        <v>0.0</v>
-      </c>
-      <c r="O8">
-        <v>0.0</v>
-      </c>
-      <c r="P8" s="24">
-        <v>31.25</v>
-      </c>
-      <c r="Q8">
-        <v>0.0</v>
-      </c>
-      <c r="R8">
-        <v>0.0</v>
-      </c>
-      <c r="S8" s="24">
-        <v>0.0</v>
-      </c>
-      <c r="T8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="23">
-        <f t="shared" si="1"/>
-        <v>43292</v>
-      </c>
-      <c r="B9" s="23">
-        <f t="shared" si="2"/>
-        <v>43657</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" t="s">
-        <v>68</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="24">
-        <v>20.75</v>
-      </c>
-      <c r="M9">
-        <v>0.0</v>
-      </c>
-      <c r="N9">
-        <v>0.0</v>
-      </c>
-      <c r="O9">
-        <v>0.0</v>
-      </c>
-      <c r="P9">
-        <v>0.0</v>
-      </c>
-      <c r="Q9">
-        <v>0.0</v>
-      </c>
-      <c r="R9">
-        <v>0.0</v>
-      </c>
-      <c r="S9" s="24">
-        <v>20.75</v>
-      </c>
-      <c r="T9">
-        <v>0.0</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1"/>
@@ -34267,11 +32822,11 @@
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="23">
         <f t="shared" ref="A2:A9" si="1">TODAY()</f>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B2" s="23">
         <f t="shared" ref="B2:B9" si="2">A2 + 365</f>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E2" t="s">
         <v>57</v>
@@ -34280,7 +32835,7 @@
         <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
         <v>59</v>
@@ -34292,7 +32847,7 @@
         <v>27</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L2" s="24">
         <v>18.75</v>
@@ -34325,11 +32880,11 @@
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B3" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E3" t="s">
         <v>61</v>
@@ -34350,7 +32905,7 @@
         <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L3">
         <v>0.0</v>
@@ -34383,11 +32938,11 @@
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B4" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E4" t="s">
         <v>63</v>
@@ -34408,7 +32963,7 @@
         <v>27</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L4" s="24">
         <v>0.0</v>
@@ -34441,11 +32996,11 @@
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B5" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -34501,11 +33056,11 @@
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B6" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E6" t="s">
         <v>57</v>
@@ -34514,7 +33069,7 @@
         <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
         <v>59</v>
@@ -34526,7 +33081,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L6" s="24">
         <v>18.75</v>
@@ -34559,11 +33114,11 @@
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B7" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E7" t="s">
         <v>61</v>
@@ -34584,7 +33139,7 @@
         <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L7">
         <v>0.0</v>
@@ -34617,11 +33172,11 @@
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B8" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
       </c>
       <c r="E8" t="s">
         <v>63</v>
@@ -34642,7 +33197,7 @@
         <v>27</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L8" s="24">
         <v>0.0</v>
@@ -34675,11 +33230,1582 @@
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="23">
         <f t="shared" si="1"/>
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="B9" s="23">
         <f t="shared" si="2"/>
-        <v>43657</v>
+        <v>43658</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L9" s="24">
+        <v>20.75</v>
+      </c>
+      <c r="M9">
+        <v>0.0</v>
+      </c>
+      <c r="N9">
+        <v>0.0</v>
+      </c>
+      <c r="O9">
+        <v>0.0</v>
+      </c>
+      <c r="P9">
+        <v>0.0</v>
+      </c>
+      <c r="Q9">
+        <v>0.0</v>
+      </c>
+      <c r="R9">
+        <v>0.0</v>
+      </c>
+      <c r="S9" s="24">
+        <v>20.75</v>
+      </c>
+      <c r="T9">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.14"/>
+    <col customWidth="1" min="2" max="2" width="18.14"/>
+    <col customWidth="1" min="3" max="3" width="13.57"/>
+    <col customWidth="1" min="4" max="4" width="16.29"/>
+    <col customWidth="1" min="5" max="5" width="17.43"/>
+    <col customWidth="1" min="6" max="6" width="5.29"/>
+    <col customWidth="1" min="7" max="7" width="11.14"/>
+    <col customWidth="1" min="8" max="8" width="12.14"/>
+    <col customWidth="1" min="9" max="9" width="11.43"/>
+    <col customWidth="1" min="10" max="10" width="11.71"/>
+    <col customWidth="1" min="11" max="11" width="15.57"/>
+    <col customWidth="1" min="12" max="13" width="5.86"/>
+    <col customWidth="1" min="14" max="14" width="3.86"/>
+    <col customWidth="1" min="15" max="15" width="5.57"/>
+    <col customWidth="1" min="16" max="16" width="10.71"/>
+    <col customWidth="1" min="17" max="17" width="5.0"/>
+    <col customWidth="1" min="18" max="18" width="12.0"/>
+    <col customWidth="1" min="19" max="19" width="9.43"/>
+    <col customWidth="1" min="20" max="20" width="4.43"/>
+    <col customWidth="1" min="21" max="21" width="12.29"/>
+    <col customWidth="1" min="22" max="22" width="13.0"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="23">
+        <f t="shared" ref="A2:A9" si="1">TODAY()</f>
+        <v>43293</v>
+      </c>
+      <c r="B2" s="23">
+        <f t="shared" ref="B2:B9" si="2">A2 + 365</f>
+        <v>43658</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="24">
+        <v>18.75</v>
+      </c>
+      <c r="M2" s="24">
+        <v>9.375</v>
+      </c>
+      <c r="N2">
+        <v>0.0</v>
+      </c>
+      <c r="O2">
+        <v>0.0</v>
+      </c>
+      <c r="P2">
+        <v>0.0</v>
+      </c>
+      <c r="Q2">
+        <v>0.0</v>
+      </c>
+      <c r="R2">
+        <v>0.0</v>
+      </c>
+      <c r="S2" s="24">
+        <v>18.75</v>
+      </c>
+      <c r="T2">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="23">
+        <f t="shared" si="1"/>
+        <v>43293</v>
+      </c>
+      <c r="B3" s="23">
+        <f t="shared" si="2"/>
+        <v>43658</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3">
+        <v>0.0</v>
+      </c>
+      <c r="M3">
+        <v>0.0</v>
+      </c>
+      <c r="N3">
+        <v>0.0</v>
+      </c>
+      <c r="O3">
+        <v>0.0</v>
+      </c>
+      <c r="P3" s="24">
+        <v>31.25</v>
+      </c>
+      <c r="Q3">
+        <v>0.0</v>
+      </c>
+      <c r="R3">
+        <v>0.0</v>
+      </c>
+      <c r="S3">
+        <v>0.0</v>
+      </c>
+      <c r="T3">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="23">
+        <f t="shared" si="1"/>
+        <v>43293</v>
+      </c>
+      <c r="B4" s="23">
+        <f t="shared" si="2"/>
+        <v>43658</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M4">
+        <v>0.0</v>
+      </c>
+      <c r="N4">
+        <v>0.0</v>
+      </c>
+      <c r="O4">
+        <v>0.0</v>
+      </c>
+      <c r="P4" s="24">
+        <v>31.25</v>
+      </c>
+      <c r="Q4">
+        <v>0.0</v>
+      </c>
+      <c r="R4">
+        <v>0.0</v>
+      </c>
+      <c r="S4" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="T4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="23">
+        <f t="shared" si="1"/>
+        <v>43293</v>
+      </c>
+      <c r="B5" s="23">
+        <f t="shared" si="2"/>
+        <v>43658</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="24">
+        <v>20.75</v>
+      </c>
+      <c r="M5">
+        <v>0.0</v>
+      </c>
+      <c r="N5">
+        <v>0.0</v>
+      </c>
+      <c r="O5">
+        <v>0.0</v>
+      </c>
+      <c r="P5">
+        <v>0.0</v>
+      </c>
+      <c r="Q5">
+        <v>0.0</v>
+      </c>
+      <c r="R5">
+        <v>0.0</v>
+      </c>
+      <c r="S5" s="24">
+        <v>20.75</v>
+      </c>
+      <c r="T5">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="23">
+        <f t="shared" si="1"/>
+        <v>43293</v>
+      </c>
+      <c r="B6" s="23">
+        <f t="shared" si="2"/>
+        <v>43658</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="24">
+        <v>18.75</v>
+      </c>
+      <c r="M6" s="24">
+        <v>9.375</v>
+      </c>
+      <c r="N6">
+        <v>0.0</v>
+      </c>
+      <c r="O6">
+        <v>0.0</v>
+      </c>
+      <c r="P6">
+        <v>0.0</v>
+      </c>
+      <c r="Q6">
+        <v>0.0</v>
+      </c>
+      <c r="R6">
+        <v>0.0</v>
+      </c>
+      <c r="S6" s="24">
+        <v>18.75</v>
+      </c>
+      <c r="T6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="23">
+        <f t="shared" si="1"/>
+        <v>43293</v>
+      </c>
+      <c r="B7" s="23">
+        <f t="shared" si="2"/>
+        <v>43658</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7">
+        <v>0.0</v>
+      </c>
+      <c r="M7">
+        <v>0.0</v>
+      </c>
+      <c r="N7">
+        <v>0.0</v>
+      </c>
+      <c r="O7">
+        <v>0.0</v>
+      </c>
+      <c r="P7" s="24">
+        <v>31.25</v>
+      </c>
+      <c r="Q7">
+        <v>0.0</v>
+      </c>
+      <c r="R7">
+        <v>0.0</v>
+      </c>
+      <c r="S7">
+        <v>0.0</v>
+      </c>
+      <c r="T7">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="23">
+        <f t="shared" si="1"/>
+        <v>43293</v>
+      </c>
+      <c r="B8" s="23">
+        <f t="shared" si="2"/>
+        <v>43658</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M8">
+        <v>0.0</v>
+      </c>
+      <c r="N8">
+        <v>0.0</v>
+      </c>
+      <c r="O8">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="24">
+        <v>31.25</v>
+      </c>
+      <c r="Q8">
+        <v>0.0</v>
+      </c>
+      <c r="R8">
+        <v>0.0</v>
+      </c>
+      <c r="S8" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="T8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="23">
+        <f t="shared" si="1"/>
+        <v>43293</v>
+      </c>
+      <c r="B9" s="23">
+        <f t="shared" si="2"/>
+        <v>43658</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>

</xml_diff>